<commit_message>
minor changes in conconi excel
</commit_message>
<xml_diff>
--- a/poznamky/conconi-test/14022016/140220016-conconi-elite.xlsx
+++ b/poznamky/conconi-test/14022016/140220016-conconi-elite.xlsx
@@ -329,11 +329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:axId val="-2072421992"/>
         <c:axId val="-2130669112"/>
-        <c:axId val="-2130358584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2130669112"/>
+        <c:axId val="-2072421992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -343,12 +343,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130358584"/>
+        <c:crossAx val="-2130669112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2130358584"/>
+        <c:axId val="-2130669112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,7 +359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130669112"/>
+        <c:crossAx val="-2072421992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17767,11 +17767,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2056646872"/>
-        <c:axId val="-2056642616"/>
+        <c:axId val="-2072089480"/>
+        <c:axId val="-2129964280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2056646872"/>
+        <c:axId val="-2072089480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17781,12 +17781,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2056642616"/>
+        <c:crossAx val="-2129964280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2056642616"/>
+        <c:axId val="-2129964280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17797,7 +17797,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2056646872"/>
+        <c:crossAx val="-2072089480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18139,8 +18139,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2080017400"/>
-        <c:axId val="-2130215128"/>
+        <c:axId val="-2079841128"/>
+        <c:axId val="-2072653048"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -18235,11 +18235,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2080017400"/>
-        <c:axId val="-2130215128"/>
+        <c:axId val="-2079841128"/>
+        <c:axId val="-2072653048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2080017400"/>
+        <c:axId val="-2079841128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60.0"/>
@@ -18251,13 +18251,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130215128"/>
+        <c:crossAx val="-2072653048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2130215128"/>
+        <c:axId val="-2072653048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="110.0"/>
@@ -18270,7 +18270,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080017400"/>
+        <c:crossAx val="-2079841128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>